<commit_message>
More work on performance results.
</commit_message>
<xml_diff>
--- a/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
+++ b/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9495"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9495" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RCP Timings Chart" sheetId="5" r:id="rId1"/>
-    <sheet name="RCP Raw Timings" sheetId="6" r:id="rId2"/>
-    <sheet name="RCP GCC" sheetId="3" r:id="rId3"/>
-    <sheet name="RCP ICC" sheetId="2" r:id="rId4"/>
-    <sheet name="RCP MSVC" sheetId="1" r:id="rId5"/>
+    <sheet name="RCP Alloc Chart" sheetId="8" r:id="rId2"/>
+    <sheet name="RCP Timings" sheetId="6" r:id="rId3"/>
+    <sheet name="RCP GCC" sheetId="3" r:id="rId4"/>
+    <sheet name="RCP ICC" sheetId="2" r:id="rId5"/>
+    <sheet name="RCP MSVC" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="Teuchos_RCP_PerformanceTest" localSheetId="3">'RCP ICC'!$A$1:$A$93</definedName>
-    <definedName name="Teuchos_RCP_PerformanceTest" localSheetId="4">'RCP MSVC'!$A$1:$A$93</definedName>
+    <definedName name="Teuchos_RCP_PerformanceTest" localSheetId="4">'RCP ICC'!$A$1:$A$93</definedName>
+    <definedName name="Teuchos_RCP_PerformanceTest" localSheetId="5">'RCP MSVC'!$A$1:$A$93</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="74">
   <si>
     <t>***</t>
   </si>
@@ -229,9 +230,6 @@
     <t>Deref</t>
   </si>
   <si>
-    <t>Member</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
@@ -241,6 +239,9 @@
     <t>Assign</t>
   </si>
   <si>
+    <t>GCC 4.1.2</t>
+  </si>
+  <si>
     <t>ICC 10.1</t>
   </si>
   <si>
@@ -248,6 +249,21 @@
   </si>
   <si>
     <t>MSVC++ 2009</t>
+  </si>
+  <si>
+    <t>ArrowOp</t>
+  </si>
+  <si>
+    <t>Alloc/Dealloc for objSize = 1</t>
+  </si>
+  <si>
+    <t>Alloc/Dealloc realtive to raw</t>
+  </si>
+  <si>
+    <t>objectSize</t>
+  </si>
+  <si>
+    <t>Zero overhead</t>
   </si>
 </sst>
 </file>
@@ -320,7 +336,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$4</c:f>
+              <c:f>'RCP Timings'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -331,14 +347,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$3:$D$3</c:f>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -348,7 +364,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$4:$D$4</c:f>
+              <c:f>'RCP Timings'!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -370,7 +386,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$5</c:f>
+              <c:f>'RCP Timings'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -381,14 +397,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$3:$D$3</c:f>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -398,7 +414,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$5:$D$5</c:f>
+              <c:f>'RCP Timings'!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -420,7 +436,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$6</c:f>
+              <c:f>'RCP Timings'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -431,14 +447,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$3:$D$3</c:f>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -448,7 +464,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$6:$D$6</c:f>
+              <c:f>'RCP Timings'!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -489,6 +505,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -541,7 +575,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$10</c:f>
+              <c:f>'RCP Timings'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -552,14 +586,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$9:$D$9</c:f>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -569,7 +603,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$10:$D$10</c:f>
+              <c:f>'RCP Timings'!$B$10:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -591,7 +625,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$11</c:f>
+              <c:f>'RCP Timings'!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -602,14 +636,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$9:$D$9</c:f>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -619,7 +653,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$11:$D$11</c:f>
+              <c:f>'RCP Timings'!$B$11:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -641,7 +675,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$12</c:f>
+              <c:f>'RCP Timings'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -652,14 +686,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$9:$D$9</c:f>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -669,7 +703,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$12:$D$12</c:f>
+              <c:f>'RCP Timings'!$B$12:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -710,6 +744,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -762,7 +814,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$16</c:f>
+              <c:f>'RCP Timings'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -773,14 +825,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$15:$D$15</c:f>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -790,7 +842,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$16:$D$16</c:f>
+              <c:f>'RCP Timings'!$B$16:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -812,7 +864,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$17</c:f>
+              <c:f>'RCP Timings'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -823,14 +875,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$15:$D$15</c:f>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -840,7 +892,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$17:$D$17</c:f>
+              <c:f>'RCP Timings'!$B$17:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -862,7 +914,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$A$18</c:f>
+              <c:f>'RCP Timings'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -873,14 +925,14 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'RCP Raw Timings'!$B$15:$D$15</c:f>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Deref</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Member</c:v>
+                  <c:v>ArrowOp</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Assign</c:v>
@@ -890,7 +942,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RCP Raw Timings'!$B$18:$D$18</c:f>
+              <c:f>'RCP Timings'!$B$18:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -930,6 +982,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -955,6 +1025,708 @@
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17064495941566024"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.68670365492569652"/>
+          <c:h val="0.71026210265383494"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$21:$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ICC 10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MSVC++ 2009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.4074620000000005E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.157942E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6285909999999998E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$21:$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ICC 10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MSVC++ 2009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$23:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.215497E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.941906E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.641363E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RCP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$21:$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ICC 10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MSVC++ 2009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$24:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.398462E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0413790000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1174530000000001E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="94251264"/>
+        <c:axId val="101491456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="94251264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101491456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="101491456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94251264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17671572855513201"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.57701807592072196"/>
+          <c:h val="0.61303988043161273"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$C$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.1.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$A$28:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$C$28:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.6409088565017274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6635825528194206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5992154756297281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4052219094889065</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1759530036907346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1090813109727911</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0359068265932216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0107305425901125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0040614077176335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ICC 10.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$A$28:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$D$28:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.7629371764734332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7002625963809082</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7536691620494176</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6386595064330598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.280041668068433</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2368421611777949</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0733737258023466</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0213468607064271</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.009381379295619</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$E$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSVC++ 2009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$A$28:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$E$28:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.5664106740074817</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7276507519980997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7318179403512215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6170214537568275</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3829787577483061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1515153069283774</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0303030116565666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0285711143428313</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zero overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$A$28:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$28:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="101493376"/>
+        <c:axId val="94382720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101493376"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>objectSize</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94382720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94382720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU time relative to raw new/delete</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101493376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1226,6 +1998,291 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="2438399"/>
+          <a:ext cx="4067175" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>a) Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to dynamically alloc and dealloc std::vector&lt;double&gt;(1)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="5295899"/>
+          <a:ext cx="5048250" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>b) Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to dynamically alloc and dealloc std::vector&lt;double&gt;(objectSize) using RCP</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1523,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1537,15 +2594,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:E39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -1558,15 +2635,15 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1">
         <f>'RCP GCC'!$C$43</f>
@@ -1583,7 +2660,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1">
         <f>'RCP GCC'!$D$43</f>
@@ -1625,15 +2702,15 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1">
         <f>'RCP ICC'!$C$43</f>
@@ -1650,7 +2727,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1">
         <f>'RCP ICC'!$D$43</f>
@@ -1692,15 +2769,15 @@
         <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1">
         <f>'RCP MSVC'!$C$43</f>
@@ -1715,9 +2792,9 @@
         <v>1.442698E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1">
         <f>'RCP MSVC'!$D$43</f>
@@ -1732,7 +2809,7 @@
         <v>4.1838250000000001E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1747,6 +2824,290 @@
       <c r="D18" s="1">
         <f>'RCP MSVC'!$E$78</f>
         <v>1.269575E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1">
+        <f>'RCP GCC'!$C$21</f>
+        <v>7.4074620000000005E-8</v>
+      </c>
+      <c r="C22" s="1">
+        <f>'RCP ICC'!$C$21</f>
+        <v>1.157942E-7</v>
+      </c>
+      <c r="D22" s="1">
+        <f>'RCP MSVC'!$C$21</f>
+        <v>2.6285909999999998E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1">
+        <f>'RCP GCC'!$D$21</f>
+        <v>1.215497E-7</v>
+      </c>
+      <c r="C23" s="1">
+        <f>'RCP ICC'!$D$21</f>
+        <v>1.941906E-7</v>
+      </c>
+      <c r="D23" s="1">
+        <f>'RCP MSVC'!$D$21</f>
+        <v>3.641363E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <f>'RCP GCC'!$E$21</f>
+        <v>1.398462E-7</v>
+      </c>
+      <c r="C24" s="1">
+        <f>'RCP ICC'!$E$21</f>
+        <v>2.0413790000000001E-7</v>
+      </c>
+      <c r="D24" s="1">
+        <f>'RCP MSVC'!$E$21</f>
+        <v>4.1174530000000001E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <f>'RCP GCC'!A21</f>
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <f>'RCP GCC'!D21/'RCP GCC'!C21</f>
+        <v>1.6409088565017274</v>
+      </c>
+      <c r="D28" s="1">
+        <f>'RCP ICC'!E21/'RCP ICC'!C21</f>
+        <v>1.7629371764734332</v>
+      </c>
+      <c r="E28" s="1">
+        <f>'RCP MSVC'!E21/'RCP MSVC'!C21</f>
+        <v>1.5664106740074817</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <f>'RCP GCC'!A22</f>
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <f>'RCP GCC'!D22/'RCP GCC'!C22</f>
+        <v>1.6635825528194206</v>
+      </c>
+      <c r="D29" s="1">
+        <f>'RCP ICC'!E22/'RCP ICC'!C22</f>
+        <v>1.7002625963809082</v>
+      </c>
+      <c r="E29" s="1">
+        <f>'RCP MSVC'!E22/'RCP MSVC'!C22</f>
+        <v>1.7276507519980997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <f>'RCP GCC'!A23</f>
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <f>'RCP GCC'!D23/'RCP GCC'!C23</f>
+        <v>1.5992154756297281</v>
+      </c>
+      <c r="D30" s="1">
+        <f>'RCP ICC'!E23/'RCP ICC'!C23</f>
+        <v>1.7536691620494176</v>
+      </c>
+      <c r="E30" s="1">
+        <f>'RCP MSVC'!E23/'RCP MSVC'!C23</f>
+        <v>1.7318179403512215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <f>'RCP GCC'!A24</f>
+        <v>64</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <f>'RCP GCC'!D24/'RCP GCC'!C24</f>
+        <v>1.4052219094889065</v>
+      </c>
+      <c r="D31" s="1">
+        <f>'RCP ICC'!E24/'RCP ICC'!C24</f>
+        <v>1.6386595064330598</v>
+      </c>
+      <c r="E31" s="1">
+        <f>'RCP MSVC'!E24/'RCP MSVC'!C24</f>
+        <v>1.6170214537568275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <f>'RCP GCC'!A25</f>
+        <v>256</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <f>'RCP GCC'!D25/'RCP GCC'!C25</f>
+        <v>1.1759530036907346</v>
+      </c>
+      <c r="D32" s="1">
+        <f>'RCP ICC'!E25/'RCP ICC'!C25</f>
+        <v>1.280041668068433</v>
+      </c>
+      <c r="E32" s="1">
+        <f>'RCP MSVC'!E25/'RCP MSVC'!C25</f>
+        <v>1.3829787577483061</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <f>'RCP GCC'!A26</f>
+        <v>1024</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <f>'RCP GCC'!D26/'RCP GCC'!C26</f>
+        <v>1.1090813109727911</v>
+      </c>
+      <c r="D33" s="1">
+        <f>'RCP ICC'!E26/'RCP ICC'!C26</f>
+        <v>1.2368421611777949</v>
+      </c>
+      <c r="E33" s="1">
+        <f>'RCP MSVC'!E26/'RCP MSVC'!C26</f>
+        <v>1.1515153069283774</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <f>'RCP GCC'!A27</f>
+        <v>4096</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <f>'RCP GCC'!D27/'RCP GCC'!C27</f>
+        <v>1.0359068265932216</v>
+      </c>
+      <c r="D34" s="1">
+        <f>'RCP ICC'!E27/'RCP ICC'!C27</f>
+        <v>1.0733737258023466</v>
+      </c>
+      <c r="E34" s="1">
+        <f>'RCP MSVC'!E27/'RCP MSVC'!C27</f>
+        <v>1.0303030116565666</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <f>'RCP GCC'!A28</f>
+        <v>16384</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <f>'RCP GCC'!D28/'RCP GCC'!C28</f>
+        <v>1.0107305425901125</v>
+      </c>
+      <c r="D35" s="1">
+        <f>'RCP ICC'!E28/'RCP ICC'!C28</f>
+        <v>1.0213468607064271</v>
+      </c>
+      <c r="E35" s="1">
+        <f>'RCP MSVC'!E28/'RCP MSVC'!C28</f>
+        <v>1.0285711143428313</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <f>'RCP GCC'!A29</f>
+        <v>65536</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <f>'RCP GCC'!D29/'RCP GCC'!C29</f>
+        <v>1.0040614077176335</v>
+      </c>
+      <c r="D36" s="1">
+        <f>'RCP ICC'!E29/'RCP ICC'!C29</f>
+        <v>1.009381379295619</v>
+      </c>
+      <c r="E36" s="1">
+        <f>'RCP MSVC'!E29/'RCP MSVC'!C29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="str">
+        <f>'RCP GCC'!A32</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
@@ -1754,12 +3115,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2812,12 +4173,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3871,12 +5232,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Finsihed RCP timing section and adding Array timing raw results.
</commit_message>
<xml_diff>
--- a/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
+++ b/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9495" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="RCP Timings Chart" sheetId="5" r:id="rId1"/>
-    <sheet name="RCP Alloc Chart" sheetId="8" r:id="rId2"/>
+    <sheet name="RCP Alloc Chart" sheetId="8" r:id="rId1"/>
+    <sheet name="RCP Timings Chart" sheetId="5" r:id="rId2"/>
     <sheet name="RCP Timings" sheetId="6" r:id="rId3"/>
     <sheet name="RCP GCC" sheetId="3" r:id="rId4"/>
     <sheet name="RCP ICC" sheetId="2" r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="75">
   <si>
     <t>***</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Zero overhead</t>
+  </si>
+  <si>
+    <t>MSVC++ 2008</t>
   </si>
 </sst>
 </file>
@@ -322,722 +325,6 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18632174103237092"/>
-          <c:y val="6.8167468649752108E-2"/>
-          <c:w val="0.68769356955380578"/>
-          <c:h val="0.7073840769903762"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$4:$D$4</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.1178119999999997E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1151580000000005E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.9191810000000004E-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$5:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>8.2385720000000002E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.325987E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.224365E-9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RCP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$6:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.1257459999999997E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.242242E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.5891580000000004E-9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="88557440"/>
-        <c:axId val="88558976"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="88557440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88558976"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="88558976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000005E-8"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>CPU Time (sec)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88557440"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId1"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18632174103237095"/>
-          <c:y val="6.8167468649752108E-2"/>
-          <c:w val="0.68769356955380589"/>
-          <c:h val="0.70738407699037631"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$10:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>6.9140170000000004E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.91194E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6780410000000004E-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$11:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.8416750000000001E-9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.9246339999999995E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0506770000000003E-9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RCP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$12:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.6587470000000001E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.7416910000000005E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.7975740000000003E-9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="92398720"/>
-        <c:axId val="92400256"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="92398720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92400256"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="92400256"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000005E-8"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>CPU Time (sec)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92398720"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId1"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18632174103237098"/>
-          <c:y val="6.8167468649752108E-2"/>
-          <c:w val="0.68769356955380601"/>
-          <c:h val="0.70738407699037642"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$16:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.035711E-9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.032826E-9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.442698E-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$17:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.0385960000000001E-9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0385960000000001E-9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1838250000000001E-9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RCP Timings'!$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RCP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Deref</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ArrowOp</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Assign</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RCP Timings'!$B$18:$D$18</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>6.9528200000000002E-10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.9239699999999998E-10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.269575E-8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="93144192"/>
-        <c:axId val="101496704"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="93144192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101496704"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="101496704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>CPU Time (sec)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93144192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
-    <c:pageSetup orientation="portrait"/>
-  </c:printSettings>
-  <c:userShapes r:id="rId1"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
           <c:x val="0.17064495941566024"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.68670365492569652"/>
@@ -1073,7 +360,7 @@
                   <c:v>ICC 10.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MSVC++ 2009</c:v>
+                  <c:v>MSVC++ 2008</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1123,7 +410,7 @@
                   <c:v>ICC 10.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MSVC++ 2009</c:v>
+                  <c:v>MSVC++ 2008</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1173,7 +460,7 @@
                   <c:v>ICC 10.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MSVC++ 2009</c:v>
+                  <c:v>MSVC++ 2008</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1267,7 +554,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1468,7 +755,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSVC++ 2009</c:v>
+                  <c:v>MSVC++ 2008</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1730,277 +1017,723 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18632174103237092"/>
+          <c:y val="6.8167468649752108E-2"/>
+          <c:w val="0.68769356955380578"/>
+          <c:h val="0.7073840769903762"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.1178119999999997E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1151580000000005E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9191810000000004E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.2385720000000002E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.325987E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.224365E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RCP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.1257459999999997E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.242242E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5891580000000004E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="88557440"/>
+        <c:axId val="88558976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="88557440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88558976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88558976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000005E-8"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88557440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.375</cdr:x>
-      <cdr:y>0.87847</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.5875</cdr:x>
-      <cdr:y>0.98264</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1714500" y="2409825"/>
-          <a:ext cx="971550" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>a) GCC</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> 4.1.2</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18632174103237095"/>
+          <c:y val="6.8167468649752108E-2"/>
+          <c:w val="0.68769356955380589"/>
+          <c:h val="0.70738407699037631"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$10:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.9140170000000004E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.91194E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6780410000000004E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.8416750000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9246339999999995E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0506770000000003E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RCP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$9:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$12:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.6587470000000001E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7416910000000005E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7975740000000003E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="92398720"/>
+        <c:axId val="92400256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="92398720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92400256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92400256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000005E-8"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92398720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.375</cdr:x>
-      <cdr:y>0.87847</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.5875</cdr:x>
-      <cdr:y>0.98264</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1714500" y="2409825"/>
-          <a:ext cx="971550" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>b) ICC </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>10.1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.375</cdr:x>
-      <cdr:y>0.87847</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.5875</cdr:x>
-      <cdr:y>0.98264</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1714500" y="2409825"/>
-          <a:ext cx="971550" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>b) ICC </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>10.1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18632174103237098"/>
+          <c:y val="6.8167468649752108E-2"/>
+          <c:w val="0.68769356955380601"/>
+          <c:h val="0.70738407699037642"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$16:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.035711E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.032826E-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.442698E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$17:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0385960000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0385960000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1838250000000001E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RCP Timings'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RCP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RCP Timings'!$B$15:$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Deref</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ArrowOp</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RCP Timings'!$B$18:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.9528200000000002E-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9239699999999998E-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.269575E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="93144192"/>
+        <c:axId val="101496704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93144192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101496704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="101496704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93144192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.375</cdr:x>
-      <cdr:y>0.87847</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.5875</cdr:x>
-      <cdr:y>0.98264</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1714500" y="2409825"/>
-          <a:ext cx="971550" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>c)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>  MSVC++ 2009</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2283,6 +2016,276 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.375</cdr:x>
+      <cdr:y>0.87847</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.5875</cdr:x>
+      <cdr:y>0.98264</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1714500" y="2409825"/>
+          <a:ext cx="971550" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>a) GCC</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> 4.1.2</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.375</cdr:x>
+      <cdr:y>0.87847</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.5875</cdr:x>
+      <cdr:y>0.98264</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1714500" y="2409825"/>
+          <a:ext cx="971550" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>b) ICC </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>10.1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.375</cdr:x>
+      <cdr:y>0.87847</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.5875</cdr:x>
+      <cdr:y>0.98264</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1714500" y="2409825"/>
+          <a:ext cx="971550" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>b) ICC </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>10.1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.375</cdr:x>
+      <cdr:y>0.87847</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.5875</cdr:x>
+      <cdr:y>0.98264</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1714500" y="2409825"/>
+          <a:ext cx="971550" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>c)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  MSVC++ 2008</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2580,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2596,8 +2599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2613,7 +2616,7 @@
   <dimension ref="A2:E39"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2839,7 +2842,7 @@
         <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2912,7 +2915,7 @@
         <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5">

</xml_diff>

<commit_message>
More progress, moved some stuff around.
</commit_message>
<xml_diff>
--- a/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
+++ b/doc/TeuchosMemoryManagementSAND/results/UnitTimings/UnitTestsResults.xlsx
@@ -1524,7 +1524,7 @@
         <c:axId val="71485312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000005E-8"/>
+          <c:max val="1.4000000000000005E-8"/>
           <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -1766,7 +1766,7 @@
         <c:axId val="64996096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000005E-8"/>
+          <c:max val="1.4000000000000005E-8"/>
           <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -7728,7 +7728,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11426,8 +11426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N29" sqref="N28:N29"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11680,8 +11680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>